<commit_message>
BW-135:Fixed Inventory Adjustment Import Module and Testing
</commit_message>
<xml_diff>
--- a/stock_inventory_import/sample file/inventory_product.xlsx
+++ b/stock_inventory_import/sample file/inventory_product.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/system/Documents/MMK/Odoo-8/sarpaylawka/2016-05-03/book_shop/addons/stock_inventory_import/sample file/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dev\Documents\bitbucket\odoo8_dms\stock_inventory_import\sample file\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11060" yWindow="5120" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,24 +24,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>default_code</t>
-  </si>
-  <si>
-    <t>balance_qty</t>
-  </si>
-  <si>
-    <t>1970205</t>
-  </si>
-  <si>
-    <t>1990002</t>
-  </si>
-  <si>
-    <t>1150024</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>uom</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>real quantity</t>
+  </si>
+  <si>
+    <t>serial number</t>
+  </si>
+  <si>
+    <t>theoretical quantity</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>pack</t>
+  </si>
+  <si>
+    <t>serial</t>
+  </si>
+  <si>
+    <t>DSP0012N</t>
+  </si>
+  <si>
+    <t>B43G</t>
+  </si>
+  <si>
+    <t>'Pcs</t>
   </si>
 </sst>
 </file>
@@ -77,9 +92,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -89,6 +105,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -357,50 +376,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="A5:B5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11" style="2"/>
+    <col min="3" max="3" width="39.25" customWidth="1"/>
+    <col min="5" max="5" width="24.625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C2">
+        <v>-10</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>20</v>
-      </c>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
   </sheetData>

</xml_diff>